<commit_message>
Adjust (de)comYear to Year(De)Com & (E)xcl(.) in PowerNetwork -> v0.0.4r
</commit_message>
<xml_diff>
--- a/examples/Power_Network.xlsx
+++ b/examples/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\InOutModule\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C160911-F528-4AB1-A693-AC290F64F608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C376D25A-F886-417A-9510-5D298BC56783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarioA" sheetId="110" r:id="rId1"/>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="103">
   <si>
     <t>[MW]</t>
   </si>
@@ -391,12 +391,6 @@
     <t>i</t>
   </si>
   <si>
-    <t>comYear</t>
-  </si>
-  <si>
-    <t>decomYear</t>
-  </si>
-  <si>
     <t>dataPackage</t>
   </si>
   <si>
@@ -553,13 +547,22 @@
     <t>Year where it is de-commissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>[0, 1]</t>
   </si>
   <si>
     <t xml:space="preserve">Whether line exists (0) or can be invested in (1) </t>
+  </si>
+  <si>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>YearCom</t>
+  </si>
+  <si>
+    <t>YearDecom</t>
   </si>
 </sst>
 </file>
@@ -1227,19 +1230,19 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>30</v>
@@ -1251,22 +1254,22 @@
         <v>3</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>31</v>
@@ -1286,7 +1289,7 @@
     </row>
     <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>43</v>
@@ -1295,181 +1298,181 @@
         <v>44</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>81</v>
-      </c>
       <c r="P4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="S4" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>74</v>
-      </c>
       <c r="I5" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="P5" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="M6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
@@ -1490,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>5</v>
@@ -1508,10 +1511,10 @@
         <v>16</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1563,10 +1566,10 @@
         <v>2029</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1621,10 +1624,10 @@
         <v>2029</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1679,10 +1682,10 @@
         <v>2029</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1737,10 +1740,10 @@
         <v>2029</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S11" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1795,10 +1798,10 @@
         <v>2050</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S12" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1853,10 +1856,10 @@
         <v>2050</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S13" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1911,10 +1914,10 @@
         <v>2050</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1969,10 +1972,10 @@
         <v>2050</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S15" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -2027,10 +2030,10 @@
         <v>2050</v>
       </c>
       <c r="R16" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S16" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -2085,10 +2088,10 @@
         <v>2050</v>
       </c>
       <c r="R17" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S17" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -2143,10 +2146,10 @@
         <v>2050</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
@@ -2201,10 +2204,10 @@
         <v>2050</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S19" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -2256,10 +2259,10 @@
         <v>2050</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S20" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -2274,7 +2277,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" s="23">
         <v>6.0000000000000001E-3</v>
@@ -2313,10 +2316,10 @@
         <v>2050</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S21" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2336,11 +2339,10 @@
   </sheetPr>
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="E38" sqref="E38"/>
-      <selection pane="topRight" activeCell="E38" sqref="E38"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
@@ -2392,19 +2394,19 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>30</v>
@@ -2416,22 +2418,22 @@
         <v>3</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>31</v>
@@ -2451,7 +2453,7 @@
     </row>
     <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>43</v>
@@ -2460,181 +2462,181 @@
         <v>44</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>75</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>81</v>
-      </c>
       <c r="P4" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="S4" s="13" t="s">
         <v>46</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>74</v>
-      </c>
       <c r="I5" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="O5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="P5" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="18"/>
       <c r="B6" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>53</v>
-      </c>
       <c r="M6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
@@ -2655,7 +2657,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>5</v>
@@ -2673,10 +2675,10 @@
         <v>16</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -2728,10 +2730,10 @@
         <v>2029</v>
       </c>
       <c r="R8" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S8" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -2786,10 +2788,10 @@
         <v>2029</v>
       </c>
       <c r="R9" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S9" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -2844,10 +2846,10 @@
         <v>2029</v>
       </c>
       <c r="R10" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S10" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -2902,10 +2904,10 @@
         <v>2029</v>
       </c>
       <c r="R11" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S11" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -2960,10 +2962,10 @@
         <v>2035</v>
       </c>
       <c r="R12" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S12" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -3018,10 +3020,10 @@
         <v>2035</v>
       </c>
       <c r="R13" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S13" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -3076,10 +3078,10 @@
         <v>2035</v>
       </c>
       <c r="R14" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S14" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -3134,10 +3136,10 @@
         <v>2035</v>
       </c>
       <c r="R15" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S15" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -3192,10 +3194,10 @@
         <v>2035</v>
       </c>
       <c r="R16" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S16" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -3250,10 +3252,10 @@
         <v>2035</v>
       </c>
       <c r="R17" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S17" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -3308,10 +3310,10 @@
         <v>2035</v>
       </c>
       <c r="R18" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S18" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
@@ -3366,10 +3368,10 @@
         <v>2035</v>
       </c>
       <c r="R19" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S19" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -3421,10 +3423,10 @@
         <v>2035</v>
       </c>
       <c r="R20" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S20" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
@@ -3439,7 +3441,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F21" s="23">
         <v>6.0000000000000001E-3</v>
@@ -3478,10 +3480,10 @@
         <v>2035</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="S21" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.25">
@@ -3538,21 +3540,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -3698,31 +3685,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3738,4 +3716,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>